<commit_message>
sữa ngon ngữ trực tiếp trên form
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRM\05.Vs.Report\VS.Report\bin\Debug\TempleteExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481BC92-37AE-49EE-B6CC-114727193BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truong_hop_Giam" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="GiamLaoDong">Truong_hop_Giam!$A$5:$BB$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -563,7 +569,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -813,18 +819,15 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,33 +837,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1024,9 +1001,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,6 +1053,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1234,41 +1245,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="6" style="29" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="29" customWidth="1"/>
-    <col min="12" max="13" width="8" style="29" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="6" style="29" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="8" style="29" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8" style="2" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="23" customWidth="1"/>
-    <col min="23" max="23" width="14" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14" style="2" customWidth="1"/>
     <col min="24" max="24" width="31" style="5" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="2" customWidth="1"/>
     <col min="27" max="27" width="9.7109375" style="2" customWidth="1"/>
     <col min="28" max="28" width="14.140625" style="5" customWidth="1"/>
     <col min="29" max="29" width="18.28515625" style="5" customWidth="1"/>
@@ -1362,7 +1373,7 @@
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1371,16 +1382,16 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1402,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="12"/>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="10" t="s">
@@ -1404,16 +1415,16 @@
       <c r="AB2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="15"/>
+      <c r="AF2" s="16"/>
       <c r="AG2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1458,25 +1469,25 @@
     <row r="3" spans="1:54" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="21"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="24" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
         <v>23</v>
       </c>
@@ -1485,30 +1496,30 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="14" t="s">
         <v>50</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
       <c r="AJ3" s="13"/>
       <c r="AK3" s="8" t="s">
         <v>28</v>
@@ -1568,66 +1579,66 @@
     <row r="4" spans="1:54" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="21"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="27" t="s">
+      <c r="T4" s="6" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="17"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="31"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="15"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="3" t="s">
         <v>48</v>
       </c>
@@ -1664,7 +1675,7 @@
       <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
       <c r="D5" t="s">
@@ -1673,58 +1684,58 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="28" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="R5" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="S5" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="28" t="s">
+      <c r="T5" t="s">
         <v>70</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" t="s">
         <v>73</v>
       </c>
       <c r="X5" t="s">
@@ -1733,7 +1744,7 @@
       <c r="Y5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" t="s">
         <v>76</v>
       </c>
       <c r="AA5" t="s">
@@ -1823,6 +1834,7 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="N2:U2"/>
@@ -1842,7 +1854,6 @@
     <mergeCell ref="AJ2:AJ4"/>
     <mergeCell ref="AI2:AI4"/>
     <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="AT3:AT4"/>
     <mergeCell ref="AU3:AU4"/>
     <mergeCell ref="AV3:AV4"/>

</xml_diff>

<commit_message>
hướng xong code nhân sự
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRM\05.Vs.Report\VS.Report\bin\Debug\TempleteExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481BC92-37AE-49EE-B6CC-114727193BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truong_hop_Giam" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="GiamLaoDong">Truong_hop_Giam!$A$5:$BB$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -563,7 +569,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -813,18 +819,15 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,33 +837,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1024,9 +1001,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,6 +1053,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1234,41 +1245,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="6" style="29" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="29" customWidth="1"/>
-    <col min="12" max="13" width="8" style="29" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="6" style="29" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="8" style="29" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8" style="2" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="23" customWidth="1"/>
-    <col min="23" max="23" width="14" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14" style="2" customWidth="1"/>
     <col min="24" max="24" width="31" style="5" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="2" customWidth="1"/>
     <col min="27" max="27" width="9.7109375" style="2" customWidth="1"/>
     <col min="28" max="28" width="14.140625" style="5" customWidth="1"/>
     <col min="29" max="29" width="18.28515625" style="5" customWidth="1"/>
@@ -1362,7 +1373,7 @@
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1371,16 +1382,16 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1402,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="12"/>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="10" t="s">
@@ -1404,16 +1415,16 @@
       <c r="AB2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="15"/>
+      <c r="AF2" s="16"/>
       <c r="AG2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1458,25 +1469,25 @@
     <row r="3" spans="1:54" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="21"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="24" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
         <v>23</v>
       </c>
@@ -1485,30 +1496,30 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="14" t="s">
         <v>50</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
       <c r="AJ3" s="13"/>
       <c r="AK3" s="8" t="s">
         <v>28</v>
@@ -1568,66 +1579,66 @@
     <row r="4" spans="1:54" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="21"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="27" t="s">
+      <c r="T4" s="6" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="17"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="31"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="15"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="3" t="s">
         <v>48</v>
       </c>
@@ -1664,7 +1675,7 @@
       <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
       <c r="D5" t="s">
@@ -1673,58 +1684,58 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="28" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="R5" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="S5" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="28" t="s">
+      <c r="T5" t="s">
         <v>70</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" t="s">
         <v>73</v>
       </c>
       <c r="X5" t="s">
@@ -1733,7 +1744,7 @@
       <c r="Y5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" t="s">
         <v>76</v>
       </c>
       <c r="AA5" t="s">
@@ -1823,6 +1834,7 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="N2:U2"/>
@@ -1842,7 +1854,6 @@
     <mergeCell ref="AJ2:AJ4"/>
     <mergeCell ref="AI2:AI4"/>
     <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="AT3:AT4"/>
     <mergeCell ref="AU3:AU4"/>
     <mergeCell ref="AV3:AV4"/>

</xml_diff>

<commit_message>
luu file yeu cau
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRM\05.Vs.Report\VS.Report\bin\Debug\TempleteExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481BC92-37AE-49EE-B6CC-114727193BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truong_hop_Giam" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="GiamLaoDong">Truong_hop_Giam!$A$5:$BB$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -563,7 +569,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -813,18 +819,15 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,33 +837,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1024,9 +1001,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,6 +1053,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1234,41 +1245,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="6" style="29" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="29" customWidth="1"/>
-    <col min="12" max="13" width="8" style="29" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="6" style="29" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="8" style="29" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8" style="2" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="23" customWidth="1"/>
-    <col min="23" max="23" width="14" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14" style="2" customWidth="1"/>
     <col min="24" max="24" width="31" style="5" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="2" customWidth="1"/>
     <col min="27" max="27" width="9.7109375" style="2" customWidth="1"/>
     <col min="28" max="28" width="14.140625" style="5" customWidth="1"/>
     <col min="29" max="29" width="18.28515625" style="5" customWidth="1"/>
@@ -1362,7 +1373,7 @@
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1371,16 +1382,16 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1402,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="12"/>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="10" t="s">
@@ -1404,16 +1415,16 @@
       <c r="AB2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="15"/>
+      <c r="AF2" s="16"/>
       <c r="AG2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1458,25 +1469,25 @@
     <row r="3" spans="1:54" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="21"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="24" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
         <v>23</v>
       </c>
@@ -1485,30 +1496,30 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="14" t="s">
         <v>50</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
       <c r="AJ3" s="13"/>
       <c r="AK3" s="8" t="s">
         <v>28</v>
@@ -1568,66 +1579,66 @@
     <row r="4" spans="1:54" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="21"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="27" t="s">
+      <c r="T4" s="6" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="17"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="31"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="15"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="3" t="s">
         <v>48</v>
       </c>
@@ -1664,7 +1675,7 @@
       <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
       <c r="D5" t="s">
@@ -1673,58 +1684,58 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="28" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="R5" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="S5" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="28" t="s">
+      <c r="T5" t="s">
         <v>70</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" t="s">
         <v>73</v>
       </c>
       <c r="X5" t="s">
@@ -1733,7 +1744,7 @@
       <c r="Y5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" t="s">
         <v>76</v>
       </c>
       <c r="AA5" t="s">
@@ -1823,6 +1834,7 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="N2:U2"/>
@@ -1842,7 +1854,6 @@
     <mergeCell ref="AJ2:AJ4"/>
     <mergeCell ref="AI2:AI4"/>
     <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="AT3:AT4"/>
     <mergeCell ref="AU3:AU4"/>
     <mergeCell ref="AV3:AV4"/>

</xml_diff>

<commit_message>
làm xong form yêu cầu tuyển dụng
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplateGiamLaoDong.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRM\05.Vs.Report\VS.Report\bin\Debug\TempleteExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481BC92-37AE-49EE-B6CC-114727193BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truong_hop_Giam" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="GiamLaoDong">Truong_hop_Giam!$A$5:$BB$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -563,7 +569,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -813,18 +819,15 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,33 +837,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1024,9 +1001,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,6 +1053,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1234,41 +1245,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="29" customWidth="1"/>
-    <col min="10" max="10" width="6" style="29" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="29" customWidth="1"/>
-    <col min="12" max="13" width="8" style="29" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="6" style="29" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="8" style="29" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8" style="2" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="23" customWidth="1"/>
-    <col min="23" max="23" width="14" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14" style="2" customWidth="1"/>
     <col min="24" max="24" width="31" style="5" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="2" customWidth="1"/>
     <col min="27" max="27" width="9.7109375" style="2" customWidth="1"/>
     <col min="28" max="28" width="14.140625" style="5" customWidth="1"/>
     <col min="29" max="29" width="18.28515625" style="5" customWidth="1"/>
@@ -1362,7 +1373,7 @@
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1371,16 +1382,16 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1402,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="12"/>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="10" t="s">
@@ -1404,16 +1415,16 @@
       <c r="AB2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="15"/>
+      <c r="AF2" s="16"/>
       <c r="AG2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1458,25 +1469,25 @@
     <row r="3" spans="1:54" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="21"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="24" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
         <v>23</v>
       </c>
@@ -1485,30 +1496,30 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="14" t="s">
         <v>50</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="30" t="s">
+      <c r="Z3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
       <c r="AJ3" s="13"/>
       <c r="AK3" s="8" t="s">
         <v>28</v>
@@ -1568,66 +1579,66 @@
     <row r="4" spans="1:54" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="21"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="27" t="s">
+      <c r="T4" s="6" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="17"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="31"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="15"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="3" t="s">
         <v>48</v>
       </c>
@@ -1664,7 +1675,7 @@
       <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
       <c r="D5" t="s">
@@ -1673,58 +1684,58 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="28" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="R5" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="S5" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="28" t="s">
+      <c r="T5" t="s">
         <v>70</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" t="s">
         <v>73</v>
       </c>
       <c r="X5" t="s">
@@ -1733,7 +1744,7 @@
       <c r="Y5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" t="s">
         <v>76</v>
       </c>
       <c r="AA5" t="s">
@@ -1823,6 +1834,7 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="N2:U2"/>
@@ -1842,7 +1854,6 @@
     <mergeCell ref="AJ2:AJ4"/>
     <mergeCell ref="AI2:AI4"/>
     <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="AT3:AT4"/>
     <mergeCell ref="AU3:AU4"/>
     <mergeCell ref="AV3:AV4"/>

</xml_diff>